<commit_message>
LV_TMTT0048689_VerifyTheCapitalSolutionChangesImplementedOnContactObject - Mid - 27 Aug 2025
</commit_message>
<xml_diff>
--- a/TestData/LV_TMTT0048689_VerifyTheCapitalSolutionChangesImplementedOnContactObject.xlsx
+++ b/TestData/LV_TMTT0048689_VerifyTheCapitalSolutionChangesImplementedOnContactObject.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5E4F07-9F89-44E9-A641-639F5E66B5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8514E3F0-33BE-4C23-BBA0-4B7BAAEA050D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
     <sheet name="Contact" sheetId="4" r:id="rId2"/>
+    <sheet name="Industry Group" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,41 +27,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Users</t>
   </si>
   <si>
-    <t>CompanyName</t>
-  </si>
-  <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>ActivityCompany</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>(541) 754-3010</t>
-  </si>
-  <si>
-    <t>LVContact</t>
-  </si>
-  <si>
-    <t>testLVContact@email.com</t>
-  </si>
-  <si>
     <t>Admin User</t>
   </si>
   <si>
@@ -68,13 +39,37 @@
   </si>
   <si>
     <t>Thomas Bailey</t>
+  </si>
+  <si>
+    <t>HL Employee</t>
+  </si>
+  <si>
+    <t>Andy Lund</t>
+  </si>
+  <si>
+    <t>Aaron Solomon</t>
+  </si>
+  <si>
+    <t>Industry Group</t>
+  </si>
+  <si>
+    <t>--None--</t>
+  </si>
+  <si>
+    <t>FT - FinTech</t>
+  </si>
+  <si>
+    <t>Jack Truett</t>
+  </si>
+  <si>
+    <t>Mark Francis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,14 +81,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -116,18 +103,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -422,15 +409,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -441,59 +428,76 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529B57F9-1065-4F8E-9B27-E98B2AE172AB}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{C3EC0CE7-3BCB-4291-B43D-0B8DF2D80B60}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
LV_TMTT0048689_VerifyTheCapitalSolutionChangesImplementedOnContactObject - Final - 27 Aug 2025
</commit_message>
<xml_diff>
--- a/TestData/LV_TMTT0048689_VerifyTheCapitalSolutionChangesImplementedOnContactObject.xlsx
+++ b/TestData/LV_TMTT0048689_VerifyTheCapitalSolutionChangesImplementedOnContactObject.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8514E3F0-33BE-4C23-BBA0-4B7BAAEA050D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5E7043-A7E5-4A38-8B47-85749D82BCFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
     <sheet name="Contact" sheetId="4" r:id="rId2"/>
-    <sheet name="Industry Group" sheetId="5" r:id="rId3"/>
+    <sheet name="Contact Type" sheetId="6" r:id="rId3"/>
+    <sheet name="Industry Group" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Users</t>
   </si>
@@ -63,6 +64,12 @@
   </si>
   <si>
     <t>Mark Francis</t>
+  </si>
+  <si>
+    <t>Contact Type</t>
+  </si>
+  <si>
+    <t>Houlihan Employee</t>
   </si>
 </sst>
 </file>
@@ -430,8 +437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,6 +477,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4BC317A-F0B1-4939-9F7B-0A5FC713D1A1}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529B57F9-1065-4F8E-9B27-E98B2AE172AB}">
   <dimension ref="A1:A3"/>
   <sheetViews>

</xml_diff>

<commit_message>
LV_TMTT0048689_VerifyTheCapitalSolutionChangesImplementedOnContactObject - Final - 28 Aug 2025
</commit_message>
<xml_diff>
--- a/TestData/LV_TMTT0048689_VerifyTheCapitalSolutionChangesImplementedOnContactObject.xlsx
+++ b/TestData/LV_TMTT0048689_VerifyTheCapitalSolutionChangesImplementedOnContactObject.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5E7043-A7E5-4A38-8B47-85749D82BCFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500C5DA7-D576-4EEE-B679-33874520147D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29760" yWindow="960" windowWidth="21600" windowHeight="11235" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
     <sheet name="Contact" sheetId="4" r:id="rId2"/>
-    <sheet name="Contact Type" sheetId="6" r:id="rId3"/>
-    <sheet name="Industry Group" sheetId="5" r:id="rId4"/>
+    <sheet name="Logic Based" sheetId="7" r:id="rId3"/>
+    <sheet name="Contact Type" sheetId="6" r:id="rId4"/>
+    <sheet name="Industry Group" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
   <si>
     <t>Users</t>
   </si>
@@ -70,6 +71,99 @@
   </si>
   <si>
     <t>Houlihan Employee</t>
+  </si>
+  <si>
+    <t>Rob Oudman</t>
+  </si>
+  <si>
+    <t>Jan Weidner</t>
+  </si>
+  <si>
+    <t>Beltran Matos</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Contact Office</t>
+  </si>
+  <si>
+    <t>Staff Industry</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>CEU</t>
+  </si>
+  <si>
+    <t>James Jin</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>ASIA</t>
+  </si>
+  <si>
+    <t>Jenny Chen</t>
+  </si>
+  <si>
+    <t>SY</t>
+  </si>
+  <si>
+    <t>SYD</t>
+  </si>
+  <si>
+    <t>FIG</t>
+  </si>
+  <si>
+    <t>Christian Scharf</t>
+  </si>
+  <si>
+    <t>BUS</t>
+  </si>
+  <si>
+    <t>TRANS - Transportation &amp; Logistics</t>
+  </si>
+  <si>
+    <t>Brian W. Eskew</t>
+  </si>
+  <si>
+    <t>IFA - Illiquid Financial Assets</t>
+  </si>
+  <si>
+    <t>CORP - Corporate</t>
+  </si>
+  <si>
+    <t>CORP</t>
+  </si>
+  <si>
+    <t>Larry DeAngelo</t>
+  </si>
+  <si>
+    <t>Adele Frost</t>
+  </si>
+  <si>
+    <t>FT</t>
+  </si>
+  <si>
+    <t>David Ho</t>
+  </si>
+  <si>
+    <t>O&amp;G - Oil &amp; Gas</t>
+  </si>
+  <si>
+    <t>O&amp;G</t>
+  </si>
+  <si>
+    <t>GEN - General</t>
   </si>
 </sst>
 </file>
@@ -113,13 +207,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,7 +538,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,10 +577,171 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA365EF-453A-4532-9643-F2ECCD628E25}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4BC317A-F0B1-4939-9F7B-0A5FC713D1A1}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -504,7 +765,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529B57F9-1065-4F8E-9B27-E98B2AE172AB}">
   <dimension ref="A1:A3"/>
   <sheetViews>

</xml_diff>